<commit_message>
Making ajax request to YQL in search bar
</commit_message>
<xml_diff>
--- a/HW5_restful/Restful.xlsx
+++ b/HW5_restful/Restful.xlsx
@@ -201,15 +201,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>JSON</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Return the stock and detail of that company</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>q=select * from yahoo.finance.historicaldata where symbol = "YHOO" and startDate = "2009-09-11" and endDate = "2010-03-10" &amp;format=json&amp;diagnostics=true&amp;env=store%3A%2F%2Fdatatables.org%2Falltableswithkeys&amp;callback=</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>JSON</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Return the stock and detail of that company</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -636,7 +636,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -681,13 +681,13 @@
         <v>46</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="G3" t="s">
         <v>48</v>
-      </c>
-      <c r="G3" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>